<commit_message>
25.09 - didnt make fine graphics 28.09 - fixed.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -358,322 +358,322 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>9.593833850610189</v>
+        <v>-9.434244289182022</v>
       </c>
       <c r="B1" t="n">
-        <v>3.131168455929254</v>
+        <v>-1.731511670396911</v>
       </c>
       <c r="C1" t="n">
-        <v>-5.061023284227097</v>
+        <v>-5.157351555497369</v>
       </c>
       <c r="D1" t="n">
-        <v>-1.245606760142097</v>
+        <v>-8.681577198524284</v>
       </c>
       <c r="E1" t="n">
-        <v>-8.011581665053619</v>
+        <v>-4.432106207228381</v>
       </c>
       <c r="F1" t="n">
-        <v>-8.643256356615138</v>
+        <v>-2.305114595987248</v>
       </c>
       <c r="G1" t="n">
-        <v>7.751689836103004</v>
+        <v>9.178048381381782</v>
       </c>
       <c r="H1" t="n">
-        <v>-4.551539830124105</v>
+        <v>-0.8834517313638841</v>
       </c>
       <c r="I1" t="n">
-        <v>-9.812825489220071</v>
+        <v>-5.970298553776734</v>
       </c>
       <c r="J1" t="n">
-        <v>9.932559715310493</v>
+        <v>-7.583697018186037</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9.497848373635691</v>
+        <v>-5.325176964424683</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.8823446265789396</v>
+        <v>8.966402808677117</v>
       </c>
       <c r="C2" t="n">
-        <v>1.352936085520543</v>
+        <v>-6.507392814361779</v>
       </c>
       <c r="D2" t="n">
-        <v>1.307065606409644</v>
+        <v>-6.682770186924363</v>
       </c>
       <c r="E2" t="n">
-        <v>-9.302505791585272</v>
+        <v>-6.794737208697324</v>
       </c>
       <c r="F2" t="n">
-        <v>4.001407719192073</v>
+        <v>5.077565090685471</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.413094345884819</v>
+        <v>-6.136471066288893</v>
       </c>
       <c r="H2" t="n">
-        <v>6.415135772325794</v>
+        <v>-7.892829808308157</v>
       </c>
       <c r="I2" t="n">
-        <v>8.433432137595933</v>
+        <v>0.446326592865347</v>
       </c>
       <c r="J2" t="n">
-        <v>7.477426775467816</v>
+        <v>7.385254513523037</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.76800362023414</v>
+        <v>-7.728765455579831</v>
       </c>
       <c r="B3" t="n">
-        <v>8.208038188357047</v>
+        <v>-1.819542622344413</v>
       </c>
       <c r="C3" t="n">
-        <v>9.736499938150523</v>
+        <v>-1.722235305494248</v>
       </c>
       <c r="D3" t="n">
-        <v>5.511930099277933</v>
+        <v>-8.334941551492378</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.594617947467399</v>
+        <v>-7.592463576800894</v>
       </c>
       <c r="F3" t="n">
-        <v>9.560461557434991</v>
+        <v>-9.793998297898348</v>
       </c>
       <c r="G3" t="n">
-        <v>3.588073286537849</v>
+        <v>7.253023750137192</v>
       </c>
       <c r="H3" t="n">
-        <v>5.272121707770374</v>
+        <v>0.2426127660608088</v>
       </c>
       <c r="I3" t="n">
-        <v>4.764084031344087</v>
+        <v>6.919258936338121</v>
       </c>
       <c r="J3" t="n">
-        <v>9.369759116019249</v>
+        <v>-6.036710473263134</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-7.618001206988767</v>
+        <v>8.827155563409018</v>
       </c>
       <c r="B4" t="n">
-        <v>-7.901500645126955</v>
+        <v>6.037909337257297</v>
       </c>
       <c r="C4" t="n">
-        <v>2.979259605206293</v>
+        <v>5.320129849073783</v>
       </c>
       <c r="D4" t="n">
-        <v>4.975238070988224</v>
+        <v>9.701311918729846</v>
       </c>
       <c r="E4" t="n">
-        <v>2.185076470428465</v>
+        <v>-8.815005648227904</v>
       </c>
       <c r="F4" t="n">
-        <v>4.561239422012484</v>
+        <v>-9.817172529134311</v>
       </c>
       <c r="G4" t="n">
-        <v>7.731940991303823</v>
+        <v>-7.908026421908292</v>
       </c>
       <c r="H4" t="n">
-        <v>7.043475077314692</v>
+        <v>4.824126551300004</v>
       </c>
       <c r="I4" t="n">
-        <v>-8.119567240799716</v>
+        <v>-7.027791806124593</v>
       </c>
       <c r="J4" t="n">
-        <v>8.07285348227844</v>
+        <v>-2.491306720063635</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6.742412795165052</v>
+        <v>-6.73121426750294</v>
       </c>
       <c r="B5" t="n">
-        <v>9.497102857985254</v>
+        <v>-2.808040171093196</v>
       </c>
       <c r="C5" t="n">
-        <v>-6.299845008375646</v>
+        <v>-7.086339693103931</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.386266389642072</v>
+        <v>1.228091464257998</v>
       </c>
       <c r="E5" t="n">
-        <v>-6.369284290443497</v>
+        <v>-0.9276670211465525</v>
       </c>
       <c r="F5" t="n">
-        <v>3.671108654172661</v>
+        <v>1.671473569237191</v>
       </c>
       <c r="G5" t="n">
-        <v>1.642526766654839</v>
+        <v>-9.77466029340653</v>
       </c>
       <c r="H5" t="n">
-        <v>2.201545691149267</v>
+        <v>-6.577205010091392</v>
       </c>
       <c r="I5" t="n">
-        <v>3.689399968012633</v>
+        <v>6.618745210005709</v>
       </c>
       <c r="J5" t="n">
-        <v>-3.507133694177329</v>
+        <v>-2.000807535718591</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-4.854464873157305</v>
+        <v>-3.481810236909095</v>
       </c>
       <c r="B6" t="n">
-        <v>8.091653171846744</v>
+        <v>-4.387968585729666</v>
       </c>
       <c r="C6" t="n">
-        <v>-8.875370276776165</v>
+        <v>-3.014076938928854</v>
       </c>
       <c r="D6" t="n">
-        <v>-5.247619282872753</v>
+        <v>9.736224147720598</v>
       </c>
       <c r="E6" t="n">
-        <v>-7.041066233196211</v>
+        <v>7.047127096497277</v>
       </c>
       <c r="F6" t="n">
-        <v>3.707179854967448</v>
+        <v>0.08909255273151295</v>
       </c>
       <c r="G6" t="n">
-        <v>-2.030849779028343</v>
+        <v>-9.968559798721399</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.759507551512149</v>
+        <v>2.739057574324676</v>
       </c>
       <c r="I6" t="n">
-        <v>5.717745429682363</v>
+        <v>-1.877296849808783</v>
       </c>
       <c r="J6" t="n">
-        <v>-2.052471548900725</v>
+        <v>4.836437105975463</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.625806103401008</v>
+        <v>7.066770774755973</v>
       </c>
       <c r="B7" t="n">
-        <v>5.373889453748697</v>
+        <v>6.739503885585663</v>
       </c>
       <c r="C7" t="n">
-        <v>-6.995749817950836</v>
+        <v>-3.279829159023917</v>
       </c>
       <c r="D7" t="n">
-        <v>9.427367327868168</v>
+        <v>-5.264013531423172</v>
       </c>
       <c r="E7" t="n">
-        <v>-3.226714033173219</v>
+        <v>-7.812915986194399</v>
       </c>
       <c r="F7" t="n">
-        <v>7.994960829221963</v>
+        <v>9.325297050105334</v>
       </c>
       <c r="G7" t="n">
-        <v>-8.407482580444833</v>
+        <v>-5.451989424611734</v>
       </c>
       <c r="H7" t="n">
-        <v>-3.510971153751221</v>
+        <v>-3.166272850042136</v>
       </c>
       <c r="I7" t="n">
-        <v>6.42874581251705</v>
+        <v>4.623089000915567</v>
       </c>
       <c r="J7" t="n">
-        <v>-6.395313169292935</v>
+        <v>4.972073058183916</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-9.665363721446242</v>
+        <v>8.040276502489618</v>
       </c>
       <c r="B8" t="n">
-        <v>-8.051817024721849</v>
+        <v>0.2226331891597049</v>
       </c>
       <c r="C8" t="n">
-        <v>-6.788396144417979</v>
+        <v>3.929805944085524</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.587730735828226</v>
+        <v>-3.767998006730238</v>
       </c>
       <c r="E8" t="n">
-        <v>-5.876643584751713</v>
+        <v>-1.024583919706977</v>
       </c>
       <c r="F8" t="n">
-        <v>-3.784511064256495</v>
+        <v>-3.635641897542332</v>
       </c>
       <c r="G8" t="n">
-        <v>5.079994448225456</v>
+        <v>3.664739604971341</v>
       </c>
       <c r="H8" t="n">
-        <v>6.048870114501014</v>
+        <v>5.333636132304669</v>
       </c>
       <c r="I8" t="n">
-        <v>-7.931115399323636</v>
+        <v>-1.125288465396299</v>
       </c>
       <c r="J8" t="n">
-        <v>-7.502430432817802</v>
+        <v>-8.020024748656308</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8.995368542848695</v>
+        <v>3.012374391324874</v>
       </c>
       <c r="B9" t="n">
-        <v>-2.65799855983647</v>
+        <v>3.209794571130224</v>
       </c>
       <c r="C9" t="n">
-        <v>5.641374310683158</v>
+        <v>7.898836227059071</v>
       </c>
       <c r="D9" t="n">
-        <v>7.066136511492253</v>
+        <v>-7.7959912781593</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.069223188414412</v>
+        <v>2.856029163557828</v>
       </c>
       <c r="F9" t="n">
-        <v>4.228918960181812</v>
+        <v>-0.006903577698217589</v>
       </c>
       <c r="G9" t="n">
-        <v>2.539358742751148</v>
+        <v>8.826465789103754</v>
       </c>
       <c r="H9" t="n">
-        <v>-5.799859968165171</v>
+        <v>-2.923686395314757</v>
       </c>
       <c r="I9" t="n">
-        <v>1.550401450758889</v>
+        <v>0.6520012786087666</v>
       </c>
       <c r="J9" t="n">
-        <v>5.411613049996983</v>
+        <v>9.65864727392654</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.173696683896296</v>
+        <v>-5.918338880128848</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.215626127800765</v>
+        <v>-7.871603907506302</v>
       </c>
       <c r="C10" t="n">
-        <v>-5.707787643485698</v>
+        <v>-0.229694167441437</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07506343680748095</v>
+        <v>-6.039676218838088</v>
       </c>
       <c r="E10" t="n">
-        <v>9.212144228866361</v>
+        <v>-2.98172594595667</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.01798670367088917</v>
+        <v>-8.736764068012759</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8521659807456032</v>
+        <v>-3.761700933777243</v>
       </c>
       <c r="H10" t="n">
-        <v>5.873209303793384</v>
+        <v>1.125753687157101</v>
       </c>
       <c r="I10" t="n">
-        <v>1.273341798252279</v>
+        <v>-5.886862157514175</v>
       </c>
       <c r="J10" t="n">
-        <v>4.660521804327967</v>
+        <v>-4.121736795401993</v>
       </c>
     </row>
   </sheetData>
@@ -697,322 +697,322 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.3838019683789931</v>
+        <v>-7.43385357226467</v>
       </c>
       <c r="B1" t="n">
-        <v>0.3419035702578803</v>
+        <v>-7.45697647674514</v>
       </c>
       <c r="C1" t="n">
-        <v>9.157184426184578</v>
+        <v>-1.193813975521117</v>
       </c>
       <c r="D1" t="n">
-        <v>2.136709057745655</v>
+        <v>-1.944186180478273</v>
       </c>
       <c r="E1" t="n">
-        <v>4.828094373806387</v>
+        <v>-2.405337147973636</v>
       </c>
       <c r="F1" t="n">
-        <v>8.592657689172416</v>
+        <v>1.427618469985772</v>
       </c>
       <c r="G1" t="n">
-        <v>5.374627549943137</v>
+        <v>-1.233861949617069</v>
       </c>
       <c r="H1" t="n">
-        <v>2.716820822410993</v>
+        <v>-5.640003600964842</v>
       </c>
       <c r="I1" t="n">
-        <v>-1.765033817711741</v>
+        <v>-1.369001667224246</v>
       </c>
       <c r="J1" t="n">
-        <v>4.899611276281174</v>
+        <v>-0.4869295442603097</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-2.151945282965633</v>
+        <v>5.472295636920386</v>
       </c>
       <c r="B2" t="n">
-        <v>-6.176521730339828</v>
+        <v>4.246676784926883</v>
       </c>
       <c r="C2" t="n">
-        <v>6.700772889850203</v>
+        <v>-5.809212339887651</v>
       </c>
       <c r="D2" t="n">
-        <v>6.54039720138698</v>
+        <v>4.278057101905651</v>
       </c>
       <c r="E2" t="n">
-        <v>-4.566186319750671</v>
+        <v>2.528105527430014</v>
       </c>
       <c r="F2" t="n">
-        <v>6.895575397615083</v>
+        <v>3.392216798159369</v>
       </c>
       <c r="G2" t="n">
-        <v>3.314991817560241</v>
+        <v>-4.48408258441408</v>
       </c>
       <c r="H2" t="n">
-        <v>-3.717644666767351</v>
+        <v>-9.676377219338184</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.386794282695812</v>
+        <v>3.125219340412237</v>
       </c>
       <c r="J2" t="n">
-        <v>8.277169730692751</v>
+        <v>-6.913876070379494</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-8.174374442336273</v>
+        <v>6.212042674380459</v>
       </c>
       <c r="B3" t="n">
-        <v>6.358619442637867</v>
+        <v>3.243756017360376</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.745641481996965</v>
+        <v>4.393978059793124</v>
       </c>
       <c r="D3" t="n">
-        <v>-5.960669338508615</v>
+        <v>2.752178124279679</v>
       </c>
       <c r="E3" t="n">
-        <v>-8.626082768457437</v>
+        <v>-7.949537938489302</v>
       </c>
       <c r="F3" t="n">
-        <v>8.291184701044585</v>
+        <v>2.741899608224896</v>
       </c>
       <c r="G3" t="n">
-        <v>4.386260402786604</v>
+        <v>0.2210928914278814</v>
       </c>
       <c r="H3" t="n">
-        <v>6.730183754434286</v>
+        <v>7.562372688992724</v>
       </c>
       <c r="I3" t="n">
-        <v>-2.050592701603328</v>
+        <v>8.864620489083872</v>
       </c>
       <c r="J3" t="n">
-        <v>8.444578363068281</v>
+        <v>8.470213649749073</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.5461403591155563</v>
+        <v>-8.152592801984103</v>
       </c>
       <c r="B4" t="n">
-        <v>-9.255617977203395</v>
+        <v>-8.00844983866547</v>
       </c>
       <c r="C4" t="n">
-        <v>-8.532254900674062</v>
+        <v>-3.955923426014413</v>
       </c>
       <c r="D4" t="n">
-        <v>-5.397408129138219</v>
+        <v>0.6077409402633975</v>
       </c>
       <c r="E4" t="n">
-        <v>5.384855799545265</v>
+        <v>4.095854914136822</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.084096154845261</v>
+        <v>-1.997113320289447</v>
       </c>
       <c r="G4" t="n">
-        <v>9.143354981773665</v>
+        <v>-6.756496959981959</v>
       </c>
       <c r="H4" t="n">
-        <v>7.489622092033027</v>
+        <v>6.12618268424529</v>
       </c>
       <c r="I4" t="n">
-        <v>5.536856759710451</v>
+        <v>9.013327017271354</v>
       </c>
       <c r="J4" t="n">
-        <v>1.851697335858663</v>
+        <v>-8.1471544156057</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-9.256938962352748</v>
+        <v>-6.615697360874481</v>
       </c>
       <c r="B5" t="n">
-        <v>7.800025870958557</v>
+        <v>-2.5506870821091</v>
       </c>
       <c r="C5" t="n">
-        <v>8.014125481842246</v>
+        <v>1.010794328857161</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5508967076732745</v>
+        <v>8.473930697198544</v>
       </c>
       <c r="E5" t="n">
-        <v>-9.499242764878748</v>
+        <v>-3.317945584512405</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.5711962646699842</v>
+        <v>4.979249789551893</v>
       </c>
       <c r="G5" t="n">
-        <v>6.36443269156392</v>
+        <v>9.154986158182083</v>
       </c>
       <c r="H5" t="n">
-        <v>-3.704357002384806</v>
+        <v>-4.893947749521064</v>
       </c>
       <c r="I5" t="n">
-        <v>3.935696894801403</v>
+        <v>1.526935626225105</v>
       </c>
       <c r="J5" t="n">
-        <v>6.164015863094011</v>
+        <v>-0.3878280995385133</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-9.480299486603137</v>
+        <v>0.6268596822365815</v>
       </c>
       <c r="B6" t="n">
-        <v>-8.769035035713838</v>
+        <v>-0.1717497451743952</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.429863484727168</v>
+        <v>1.709992090836154</v>
       </c>
       <c r="D6" t="n">
-        <v>-7.792097080200742</v>
+        <v>-0.7915996427554575</v>
       </c>
       <c r="E6" t="n">
-        <v>1.923881649002624</v>
+        <v>-5.287584713798297</v>
       </c>
       <c r="F6" t="n">
-        <v>-6.413530647503521</v>
+        <v>3.904274045486106</v>
       </c>
       <c r="G6" t="n">
-        <v>-7.836833024384466</v>
+        <v>0.09912944754993447</v>
       </c>
       <c r="H6" t="n">
-        <v>-8.226025559968358</v>
+        <v>9.954188307607581</v>
       </c>
       <c r="I6" t="n">
-        <v>2.580251546204703</v>
+        <v>-8.693357297273669</v>
       </c>
       <c r="J6" t="n">
-        <v>1.476379642453329</v>
+        <v>0.9575797043256991</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3.110733792105018</v>
+        <v>1.993004382090788</v>
       </c>
       <c r="B7" t="n">
-        <v>7.292975760463861</v>
+        <v>-3.196547362187443</v>
       </c>
       <c r="C7" t="n">
-        <v>1.557098673725685</v>
+        <v>5.030582907392711</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.926646500627137</v>
+        <v>-7.740734407031871</v>
       </c>
       <c r="E7" t="n">
-        <v>8.288447997291438</v>
+        <v>-5.766907007419666</v>
       </c>
       <c r="F7" t="n">
-        <v>-9.852065544504727</v>
+        <v>1.320421075803161</v>
       </c>
       <c r="G7" t="n">
-        <v>4.063684595555108</v>
+        <v>-9.738926802276197</v>
       </c>
       <c r="H7" t="n">
-        <v>1.458622234607649</v>
+        <v>-6.909457526412472</v>
       </c>
       <c r="I7" t="n">
-        <v>-6.980310737877069</v>
+        <v>9.107856519409296</v>
       </c>
       <c r="J7" t="n">
-        <v>-1.730008707392658</v>
+        <v>8.216695050576174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-3.647950958604449</v>
+        <v>-2.122570391028569</v>
       </c>
       <c r="B8" t="n">
-        <v>-2.284344211391613</v>
+        <v>0.1856918657852376</v>
       </c>
       <c r="C8" t="n">
-        <v>7.290053146723757</v>
+        <v>-6.395101503052308</v>
       </c>
       <c r="D8" t="n">
-        <v>5.243845434229286</v>
+        <v>5.677619135883997</v>
       </c>
       <c r="E8" t="n">
-        <v>-3.370696076439794</v>
+        <v>9.704227732218996</v>
       </c>
       <c r="F8" t="n">
-        <v>4.755048189853493</v>
+        <v>2.330383763132884</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.006119853853868</v>
+        <v>-5.659636692531668</v>
       </c>
       <c r="H8" t="n">
-        <v>-1.797843710350149</v>
+        <v>9.926802988079519</v>
       </c>
       <c r="I8" t="n">
-        <v>-6.930766487419772</v>
+        <v>0.6071901095813317</v>
       </c>
       <c r="J8" t="n">
-        <v>7.514423324950972</v>
+        <v>-7.309250930955599</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-5.49384219660096</v>
+        <v>6.894247344037151</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.8017981997321382</v>
+        <v>3.920746647279271</v>
       </c>
       <c r="C9" t="n">
-        <v>-8.139925747568244</v>
+        <v>5.460035139311328</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1190140615202893</v>
+        <v>5.159450560785174</v>
       </c>
       <c r="E9" t="n">
-        <v>-5.613718619173252</v>
+        <v>7.520600499380205</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.217561999281942</v>
+        <v>7.128073281358603</v>
       </c>
       <c r="G9" t="n">
-        <v>6.475475792161497</v>
+        <v>-0.8985149253122025</v>
       </c>
       <c r="H9" t="n">
-        <v>-1.087882454880337</v>
+        <v>-2.164446415642363</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.3319173749621882</v>
+        <v>1.638392213654118</v>
       </c>
       <c r="J9" t="n">
-        <v>1.089233842916792</v>
+        <v>5.681729527279183</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-1.386357130809388</v>
+        <v>0.3081304858064104</v>
       </c>
       <c r="B10" t="n">
-        <v>-9.562312789407294</v>
+        <v>-8.259868233215453</v>
       </c>
       <c r="C10" t="n">
-        <v>4.44078013096269</v>
+        <v>-7.844101442279287</v>
       </c>
       <c r="D10" t="n">
-        <v>1.145660730440758</v>
+        <v>-3.267852912414345</v>
       </c>
       <c r="E10" t="n">
-        <v>-7.499101324730431</v>
+        <v>5.175142361287046</v>
       </c>
       <c r="F10" t="n">
-        <v>9.619334125807725</v>
+        <v>-7.015070378698804</v>
       </c>
       <c r="G10" t="n">
-        <v>-9.18253918133626</v>
+        <v>2.910003644362988</v>
       </c>
       <c r="H10" t="n">
-        <v>-9.108635666266089</v>
+        <v>-8.834158019983974</v>
       </c>
       <c r="I10" t="n">
-        <v>6.876591563266228</v>
+        <v>3.205183576607343</v>
       </c>
       <c r="J10" t="n">
-        <v>-5.915705351798398</v>
+        <v>0.6899828221952369</v>
       </c>
     </row>
   </sheetData>
@@ -1036,322 +1036,322 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>9.977635818989182</v>
+        <v>-16.86809786144669</v>
       </c>
       <c r="B1" t="n">
-        <v>3.473072026187134</v>
+        <v>-9.188488147142051</v>
       </c>
       <c r="C1" t="n">
-        <v>4.096161141957481</v>
+        <v>-6.351165531018486</v>
       </c>
       <c r="D1" t="n">
-        <v>0.8911022976035579</v>
+        <v>-10.62576337900256</v>
       </c>
       <c r="E1" t="n">
-        <v>-3.183487291247232</v>
+        <v>-6.837443355202018</v>
       </c>
       <c r="F1" t="n">
-        <v>-0.05059866744272234</v>
+        <v>-0.8774961260014758</v>
       </c>
       <c r="G1" t="n">
-        <v>13.12631738604614</v>
+        <v>7.944186431764713</v>
       </c>
       <c r="H1" t="n">
-        <v>-1.834719007713112</v>
+        <v>-6.523455332328727</v>
       </c>
       <c r="I1" t="n">
-        <v>-11.57785930693181</v>
+        <v>-7.339300221000981</v>
       </c>
       <c r="J1" t="n">
-        <v>14.83217099159167</v>
+        <v>-8.070626562446346</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7.345903090670058</v>
+        <v>0.1471186724957025</v>
       </c>
       <c r="B2" t="n">
-        <v>-7.058866356918768</v>
+        <v>13.213079593604</v>
       </c>
       <c r="C2" t="n">
-        <v>8.053708975370746</v>
+        <v>-12.31660515424943</v>
       </c>
       <c r="D2" t="n">
-        <v>7.847462807796624</v>
+        <v>-2.404713085018712</v>
       </c>
       <c r="E2" t="n">
-        <v>-13.86869211133594</v>
+        <v>-4.26663168126731</v>
       </c>
       <c r="F2" t="n">
-        <v>10.89698311680716</v>
+        <v>8.469781888844841</v>
       </c>
       <c r="G2" t="n">
-        <v>1.901897471675422</v>
+        <v>-10.62055365070297</v>
       </c>
       <c r="H2" t="n">
-        <v>2.697491105558443</v>
+        <v>-17.56920702764634</v>
       </c>
       <c r="I2" t="n">
-        <v>7.046637854900121</v>
+        <v>3.571545933277584</v>
       </c>
       <c r="J2" t="n">
-        <v>15.75459650616057</v>
+        <v>0.4713784431435428</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-2.406370822102133</v>
+        <v>-1.516722781199372</v>
       </c>
       <c r="B3" t="n">
-        <v>14.56665763099491</v>
+        <v>1.424213395015963</v>
       </c>
       <c r="C3" t="n">
-        <v>4.990858456153558</v>
+        <v>2.671742754298876</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.4487392392306822</v>
+        <v>-5.582763427212699</v>
       </c>
       <c r="E3" t="n">
-        <v>-11.22070071592483</v>
+        <v>-15.5420015152902</v>
       </c>
       <c r="F3" t="n">
-        <v>17.85164625847958</v>
+        <v>-7.052098689673452</v>
       </c>
       <c r="G3" t="n">
-        <v>7.974333689324453</v>
+        <v>7.474116641565073</v>
       </c>
       <c r="H3" t="n">
-        <v>12.00230546220466</v>
+        <v>7.804985455053533</v>
       </c>
       <c r="I3" t="n">
-        <v>2.713491329740759</v>
+        <v>15.78387942542199</v>
       </c>
       <c r="J3" t="n">
-        <v>17.81433747908753</v>
+        <v>2.43350317648594</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-8.164141566104323</v>
+        <v>0.6745627614249159</v>
       </c>
       <c r="B4" t="n">
-        <v>-17.15711862233035</v>
+        <v>-1.970540501408173</v>
       </c>
       <c r="C4" t="n">
-        <v>-5.552995295467769</v>
+        <v>1.36420642305937</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4221700581499945</v>
+        <v>10.30905285899324</v>
       </c>
       <c r="E4" t="n">
-        <v>7.56993226997373</v>
+        <v>-4.719150734091082</v>
       </c>
       <c r="F4" t="n">
-        <v>2.477143267167223</v>
+        <v>-11.81428584942376</v>
       </c>
       <c r="G4" t="n">
-        <v>16.87529597307749</v>
+        <v>-14.66452338189025</v>
       </c>
       <c r="H4" t="n">
-        <v>14.53309716934772</v>
+        <v>10.95030923554529</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.582710481089265</v>
+        <v>1.985535211146762</v>
       </c>
       <c r="J4" t="n">
-        <v>9.924550818137103</v>
+        <v>-10.63846113566933</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-2.514526167187697</v>
+        <v>-13.34691162837742</v>
       </c>
       <c r="B5" t="n">
-        <v>17.29712872894381</v>
+        <v>-5.358727253202296</v>
       </c>
       <c r="C5" t="n">
-        <v>1.7142804734666</v>
+        <v>-6.07554536424677</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.8353696819687979</v>
+        <v>9.702022161456542</v>
       </c>
       <c r="E5" t="n">
-        <v>-15.86852705532224</v>
+        <v>-4.245612605658957</v>
       </c>
       <c r="F5" t="n">
-        <v>3.099912389502677</v>
+        <v>6.650723358789085</v>
       </c>
       <c r="G5" t="n">
-        <v>8.006959458218759</v>
+        <v>-0.6196741352244466</v>
       </c>
       <c r="H5" t="n">
-        <v>-1.502811311235539</v>
+        <v>-11.47115275961245</v>
       </c>
       <c r="I5" t="n">
-        <v>7.625096862814036</v>
+        <v>8.145680836230815</v>
       </c>
       <c r="J5" t="n">
-        <v>2.656882168916683</v>
+        <v>-2.388635635257105</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-14.33476435976044</v>
+        <v>-2.854950554672514</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.6773818638670939</v>
+        <v>-4.559718330904062</v>
       </c>
       <c r="C6" t="n">
-        <v>-10.30523376150333</v>
+        <v>-1.3040848480927</v>
       </c>
       <c r="D6" t="n">
-        <v>-13.0397163630735</v>
+        <v>8.944624504965141</v>
       </c>
       <c r="E6" t="n">
-        <v>-5.117184584193588</v>
+        <v>1.759542382698981</v>
       </c>
       <c r="F6" t="n">
-        <v>-2.706350792536073</v>
+        <v>3.993366598217619</v>
       </c>
       <c r="G6" t="n">
-        <v>-9.867682803412809</v>
+        <v>-9.869430351171465</v>
       </c>
       <c r="H6" t="n">
-        <v>-8.985533111480507</v>
+        <v>12.69324588193226</v>
       </c>
       <c r="I6" t="n">
-        <v>8.297996975887067</v>
+        <v>-10.57065414708245</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.5760919064473953</v>
+        <v>5.794016810301162</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5.736539895506025</v>
+        <v>9.059775156846761</v>
       </c>
       <c r="B7" t="n">
-        <v>12.66686521421256</v>
+        <v>3.542956523398219</v>
       </c>
       <c r="C7" t="n">
-        <v>-5.438651144225151</v>
+        <v>1.750753748368794</v>
       </c>
       <c r="D7" t="n">
-        <v>6.500720827241032</v>
+        <v>-13.00474793845504</v>
       </c>
       <c r="E7" t="n">
-        <v>5.061733964118219</v>
+        <v>-13.57982299361407</v>
       </c>
       <c r="F7" t="n">
-        <v>-1.857104715282764</v>
+        <v>10.64571812590849</v>
       </c>
       <c r="G7" t="n">
-        <v>-4.343797984889726</v>
+        <v>-15.19091622688793</v>
       </c>
       <c r="H7" t="n">
-        <v>-2.052348919143572</v>
+        <v>-10.07573037645461</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.5515649253600188</v>
+        <v>13.73094552032486</v>
       </c>
       <c r="J7" t="n">
-        <v>-8.125321876685593</v>
+        <v>13.18876810876009</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-13.31331468005069</v>
+        <v>5.917706111461049</v>
       </c>
       <c r="B8" t="n">
-        <v>-10.33616123611346</v>
+        <v>0.4083250549449424</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5016570023057785</v>
+        <v>-2.465295558966783</v>
       </c>
       <c r="D8" t="n">
-        <v>1.65611469840106</v>
+        <v>1.909621129153759</v>
       </c>
       <c r="E8" t="n">
-        <v>-9.247339661191507</v>
+        <v>8.679643812512019</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9705371255969979</v>
+        <v>-1.305258134409447</v>
       </c>
       <c r="G8" t="n">
-        <v>4.073874594371588</v>
+        <v>-1.994897087560327</v>
       </c>
       <c r="H8" t="n">
-        <v>4.251026404150865</v>
+        <v>15.26043912038419</v>
       </c>
       <c r="I8" t="n">
-        <v>-14.86188188674341</v>
+        <v>-0.518098355814967</v>
       </c>
       <c r="J8" t="n">
-        <v>0.01199289213317023</v>
+        <v>-15.32927567961191</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.501526346247735</v>
+        <v>9.906621735362025</v>
       </c>
       <c r="B9" t="n">
-        <v>-3.459796759568608</v>
+        <v>7.130541218409496</v>
       </c>
       <c r="C9" t="n">
-        <v>-2.498551436885085</v>
+        <v>13.3588713663704</v>
       </c>
       <c r="D9" t="n">
-        <v>7.185150573012542</v>
+        <v>-2.636540717374126</v>
       </c>
       <c r="E9" t="n">
-        <v>-8.682941807587664</v>
+        <v>10.37662966293803</v>
       </c>
       <c r="F9" t="n">
-        <v>3.011356960899869</v>
+        <v>7.121169703660385</v>
       </c>
       <c r="G9" t="n">
-        <v>9.014834534912644</v>
+        <v>7.927950863791551</v>
       </c>
       <c r="H9" t="n">
-        <v>-6.887742423045507</v>
+        <v>-5.08813281095712</v>
       </c>
       <c r="I9" t="n">
-        <v>1.218484075796701</v>
+        <v>2.290393492262885</v>
       </c>
       <c r="J9" t="n">
-        <v>6.500846892913776</v>
+        <v>15.34037680120572</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.7873395530869072</v>
+        <v>-5.610208394322438</v>
       </c>
       <c r="B10" t="n">
-        <v>-11.77793891720806</v>
+        <v>-16.13147214072175</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.267007512523008</v>
+        <v>-8.073795609720724</v>
       </c>
       <c r="D10" t="n">
-        <v>1.220724167248239</v>
+        <v>-9.307529131252434</v>
       </c>
       <c r="E10" t="n">
-        <v>1.71304290413593</v>
+        <v>2.193416415330375</v>
       </c>
       <c r="F10" t="n">
-        <v>9.601347422136836</v>
+        <v>-15.75183444671156</v>
       </c>
       <c r="G10" t="n">
-        <v>-8.330373200590657</v>
+        <v>-0.8516972894142558</v>
       </c>
       <c r="H10" t="n">
-        <v>-3.235426362472705</v>
+        <v>-7.708404332826873</v>
       </c>
       <c r="I10" t="n">
-        <v>8.149933361518507</v>
+        <v>-2.681678580906832</v>
       </c>
       <c r="J10" t="n">
-        <v>-1.25518354747043</v>
+        <v>-3.431753973206757</v>
       </c>
     </row>
   </sheetData>
@@ -1375,322 +1375,322 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>275.9556632602747</v>
+        <v>103.9432085518313</v>
       </c>
       <c r="B1" t="n">
-        <v>-43.58951838187743</v>
+        <v>137.2255655026671</v>
       </c>
       <c r="C1" t="n">
-        <v>194.5054103228061</v>
+        <v>103.2920867574497</v>
       </c>
       <c r="D1" t="n">
-        <v>104.4614422277217</v>
+        <v>-126.3501025845109</v>
       </c>
       <c r="E1" t="n">
-        <v>188.639691481788</v>
+        <v>-94.99995912530281</v>
       </c>
       <c r="F1" t="n">
-        <v>134.1511853387209</v>
+        <v>-26.50982444829447</v>
       </c>
       <c r="G1" t="n">
-        <v>-73.56734017720981</v>
+        <v>-64.97129229594172</v>
       </c>
       <c r="H1" t="n">
-        <v>11.50369902513198</v>
+        <v>-15.74507678498795</v>
       </c>
       <c r="I1" t="n">
-        <v>-22.63164962280304</v>
+        <v>-54.22497942090088</v>
       </c>
       <c r="J1" t="n">
-        <v>-151.3249156189997</v>
+        <v>85.83946706342928</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-42.54720271067123</v>
+        <v>160.7217220042294</v>
       </c>
       <c r="B2" t="n">
-        <v>-205.6694409894728</v>
+        <v>85.55513759941377</v>
       </c>
       <c r="C2" t="n">
-        <v>-7.660073524284194</v>
+        <v>-81.96107235660851</v>
       </c>
       <c r="D2" t="n">
-        <v>10.4459052170869</v>
+        <v>-53.99932375016787</v>
       </c>
       <c r="E2" t="n">
-        <v>4.565547102643258</v>
+        <v>55.9035077453502</v>
       </c>
       <c r="F2" t="n">
-        <v>169.7571019667125</v>
+        <v>-70.8138751068993</v>
       </c>
       <c r="G2" t="n">
-        <v>-50.80385289179143</v>
+        <v>73.89871001313719</v>
       </c>
       <c r="H2" t="n">
-        <v>-41.35506918289412</v>
+        <v>-165.2427871073876</v>
       </c>
       <c r="I2" t="n">
-        <v>-23.34284678408159</v>
+        <v>-173.4038146960261</v>
       </c>
       <c r="J2" t="n">
-        <v>17.24695459014958</v>
+        <v>-37.67492741153048</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-211.901239339917</v>
+        <v>208.623532866504</v>
       </c>
       <c r="B3" t="n">
-        <v>-221.1967668069585</v>
+        <v>185.9692900778437</v>
       </c>
       <c r="C3" t="n">
-        <v>26.97077485388862</v>
+        <v>140.847035608188</v>
       </c>
       <c r="D3" t="n">
-        <v>-69.25650118546785</v>
+        <v>-58.48802772583032</v>
       </c>
       <c r="E3" t="n">
-        <v>-105.9379304674159</v>
+        <v>51.84353333370517</v>
       </c>
       <c r="F3" t="n">
-        <v>189.6166122562188</v>
+        <v>20.48574895129178</v>
       </c>
       <c r="G3" t="n">
-        <v>13.96573855669537</v>
+        <v>-92.64400473839717</v>
       </c>
       <c r="H3" t="n">
-        <v>-71.8397327577695</v>
+        <v>-72.57609874146439</v>
       </c>
       <c r="I3" t="n">
-        <v>4.711369032853753</v>
+        <v>46.24573661699802</v>
       </c>
       <c r="J3" t="n">
-        <v>169.9189921534789</v>
+        <v>156.1985460741975</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-44.68648236846918</v>
+        <v>-101.6763711440215</v>
       </c>
       <c r="B4" t="n">
-        <v>-34.24553054724856</v>
+        <v>-57.24983459058085</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.975428876901705</v>
+        <v>-175.7747265379647</v>
       </c>
       <c r="D4" t="n">
-        <v>-124.3174005026196</v>
+        <v>22.76540476932036</v>
       </c>
       <c r="E4" t="n">
-        <v>13.79580456284716</v>
+        <v>99.30481341237596</v>
       </c>
       <c r="F4" t="n">
-        <v>-91.25528381396471</v>
+        <v>-85.74247802638925</v>
       </c>
       <c r="G4" t="n">
-        <v>-132.7918176545398</v>
+        <v>-135.2332916278221</v>
       </c>
       <c r="H4" t="n">
-        <v>-45.70796313617605</v>
+        <v>76.62093185721044</v>
       </c>
       <c r="I4" t="n">
-        <v>21.63137181086866</v>
+        <v>124.676288682241</v>
       </c>
       <c r="J4" t="n">
-        <v>-65.20251505740451</v>
+        <v>-227.8885918721138</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>40.23325146168141</v>
+        <v>27.31900129411905</v>
       </c>
       <c r="B5" t="n">
-        <v>-127.9260597978145</v>
+        <v>80.02797546893987</v>
       </c>
       <c r="C5" t="n">
-        <v>83.81191298295377</v>
+        <v>34.99616171826582</v>
       </c>
       <c r="D5" t="n">
-        <v>92.59906036431283</v>
+        <v>52.14076365195204</v>
       </c>
       <c r="E5" t="n">
-        <v>115.4141141865714</v>
+        <v>96.66025552608016</v>
       </c>
       <c r="F5" t="n">
-        <v>10.23032185592915</v>
+        <v>-6.130324305495381</v>
       </c>
       <c r="G5" t="n">
-        <v>18.66084735776069</v>
+        <v>123.3553444685915</v>
       </c>
       <c r="H5" t="n">
-        <v>-50.00582243601648</v>
+        <v>45.84432852019071</v>
       </c>
       <c r="I5" t="n">
-        <v>-87.48889364816677</v>
+        <v>-155.845096878845</v>
       </c>
       <c r="J5" t="n">
-        <v>60.50498366983834</v>
+        <v>-41.39141239560939</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>54.06041438577716</v>
+        <v>-179.9273719317868</v>
       </c>
       <c r="B6" t="n">
-        <v>-144.9661265454068</v>
+        <v>-113.3449621821385</v>
       </c>
       <c r="C6" t="n">
-        <v>-29.42398068213076</v>
+        <v>-130.688554277114</v>
       </c>
       <c r="D6" t="n">
-        <v>91.3010268626355</v>
+        <v>112.4901877274296</v>
       </c>
       <c r="E6" t="n">
-        <v>30.95452215800874</v>
+        <v>132.246338460834</v>
       </c>
       <c r="F6" t="n">
-        <v>-78.6297713939704</v>
+        <v>-66.21612616180717</v>
       </c>
       <c r="G6" t="n">
-        <v>-111.6592041468429</v>
+        <v>119.3899418572322</v>
       </c>
       <c r="H6" t="n">
-        <v>-135.8406800572996</v>
+        <v>122.7528326784518</v>
       </c>
       <c r="I6" t="n">
-        <v>-28.22665201688481</v>
+        <v>-14.62680371212357</v>
       </c>
       <c r="J6" t="n">
-        <v>-63.22690036846292</v>
+        <v>-184.7252001042405</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-44.2423585454444</v>
+        <v>93.6812436210337</v>
       </c>
       <c r="B7" t="n">
-        <v>-256.6060103315663</v>
+        <v>19.664944187156</v>
       </c>
       <c r="C7" t="n">
-        <v>-143.8903102365442</v>
+        <v>-54.06341433869999</v>
       </c>
       <c r="D7" t="n">
-        <v>-32.86814804283414</v>
+        <v>-38.89087012187515</v>
       </c>
       <c r="E7" t="n">
-        <v>99.30245404228842</v>
+        <v>42.38170794381344</v>
       </c>
       <c r="F7" t="n">
-        <v>-70.67453865213366</v>
+        <v>15.47315716076424</v>
       </c>
       <c r="G7" t="n">
-        <v>73.96983963703751</v>
+        <v>6.629822964517992</v>
       </c>
       <c r="H7" t="n">
-        <v>2.174212886332124</v>
+        <v>-78.75161294377946</v>
       </c>
       <c r="I7" t="n">
-        <v>99.29473506034746</v>
+        <v>-186.1982952077241</v>
       </c>
       <c r="J7" t="n">
-        <v>40.63786904856417</v>
+        <v>-14.92791864760499</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>209.0556830481726</v>
+        <v>-13.16795528196013</v>
       </c>
       <c r="B8" t="n">
-        <v>125.1482914365267</v>
+        <v>38.25854249618074</v>
       </c>
       <c r="C8" t="n">
-        <v>-38.07032913030761</v>
+        <v>55.12131735621019</v>
       </c>
       <c r="D8" t="n">
-        <v>20.07837183184601</v>
+        <v>10.35889167561486</v>
       </c>
       <c r="E8" t="n">
-        <v>200.3822787914023</v>
+        <v>-62.16977958615191</v>
       </c>
       <c r="F8" t="n">
-        <v>-243.5484788945267</v>
+        <v>76.74603596519373</v>
       </c>
       <c r="G8" t="n">
-        <v>-116.8707053516719</v>
+        <v>-82.5363146722862</v>
       </c>
       <c r="H8" t="n">
-        <v>57.51739941462755</v>
+        <v>28.86852294460794</v>
       </c>
       <c r="I8" t="n">
-        <v>-136.9542072629441</v>
+        <v>29.67126414043976</v>
       </c>
       <c r="J8" t="n">
-        <v>-147.3737506425652</v>
+        <v>34.64629553370109</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-39.44452270184737</v>
+        <v>120.1659895532024</v>
       </c>
       <c r="B9" t="n">
-        <v>-92.28321953203707</v>
+        <v>-34.04013594000606</v>
       </c>
       <c r="C9" t="n">
-        <v>-80.05995461092003</v>
+        <v>37.07619781789247</v>
       </c>
       <c r="D9" t="n">
-        <v>-136.0330249180758</v>
+        <v>-64.03858844194694</v>
       </c>
       <c r="E9" t="n">
-        <v>73.5569611462025</v>
+        <v>-127.6792803806919</v>
       </c>
       <c r="F9" t="n">
-        <v>63.21555088846313</v>
+        <v>8.342826170140555</v>
       </c>
       <c r="G9" t="n">
-        <v>52.71479264892766</v>
+        <v>20.56391739186218</v>
       </c>
       <c r="H9" t="n">
-        <v>64.94492025831848</v>
+        <v>-226.8668733387766</v>
       </c>
       <c r="I9" t="n">
-        <v>73.36794422250439</v>
+        <v>120.7216430504911</v>
       </c>
       <c r="J9" t="n">
-        <v>-8.179247353952187</v>
+        <v>209.9099110304792</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-65.1179685138237</v>
+        <v>11.23984868481181</v>
       </c>
       <c r="B10" t="n">
-        <v>-3.335597301345576</v>
+        <v>90.63172154874007</v>
       </c>
       <c r="C10" t="n">
-        <v>159.8325451267887</v>
+        <v>31.78872038063317</v>
       </c>
       <c r="D10" t="n">
-        <v>62.78079892851521</v>
+        <v>-26.21627195903312</v>
       </c>
       <c r="E10" t="n">
-        <v>-72.12274777748317</v>
+        <v>-5.472098985503247</v>
       </c>
       <c r="F10" t="n">
-        <v>13.58501142556956</v>
+        <v>-88.06797913622334</v>
       </c>
       <c r="G10" t="n">
-        <v>1.763398200173156</v>
+        <v>78.75061263583503</v>
       </c>
       <c r="H10" t="n">
-        <v>-110.8392852153905</v>
+        <v>84.75620456578335</v>
       </c>
       <c r="I10" t="n">
-        <v>32.53736497845201</v>
+        <v>-58.00649142331325</v>
       </c>
       <c r="J10" t="n">
-        <v>17.48375756969665</v>
+        <v>21.92732144204887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>